<commit_message>
Dodan readme, manjši popravki
</commit_message>
<xml_diff>
--- a/primer.xlsx
+++ b/primer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomazc/workspace-git/RD-ULFRI/rd-zahtevki/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7607D1B9-61AB-1544-91DC-82B181FFA7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AC38E8-401F-344C-AEA3-A3248AEFBA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48300" yWindow="6620" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47760" yWindow="6620" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FN" sheetId="5" r:id="rId1"/>
@@ -748,7 +748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -1486,7 +1486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A121" sqref="A121"/>
     </sheetView>

</xml_diff>